<commit_message>
new -- tf Dataset,Estimator
</commit_message>
<xml_diff>
--- a/博客-文章/王喆/目录--王喆.xlsx
+++ b/博客-文章/王喆/目录--王喆.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\reference\note\博客-文章\王喆\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9CE6C9-0A16-4D0A-802C-41B5BA5BCF77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8155DCA7-AC70-44F6-A77A-A1E36E715D2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="165" windowWidth="15270" windowHeight="9840" xr2:uid="{7409FE34-15D6-B64C-BF58-D8854FBAF8E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7409FE34-15D6-B64C-BF58-D8854FBAF8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -190,6 +190,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -230,7 +238,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -238,6 +246,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,73 +568,73 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="85.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -631,12 +642,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -644,27 +655,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -672,7 +683,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -680,12 +691,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -693,98 +704,98 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>